<commit_message>
Removed webElement and replaced with Selenium By
</commit_message>
<xml_diff>
--- a/resources/locators/locators.xlsx
+++ b/resources/locators/locators.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="669" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="669" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LocatorStrategy" sheetId="31" r:id="rId1"/>
-    <sheet name="CommonLocators" sheetId="32" r:id="rId2"/>
-    <sheet name="HomePage" sheetId="30" r:id="rId3"/>
+    <sheet name="HomePage" sheetId="30" r:id="rId2"/>
+    <sheet name="UsersPage" sheetId="32" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Element Name</t>
   </si>
@@ -60,7 +60,34 @@
     <t>//a[@href='/questions/ask']</t>
   </si>
   <si>
-    <t>ask_question_button</t>
+    <t>//button[@type='submit']//*[@class='svg-icon iconSearch']</t>
+  </si>
+  <si>
+    <t>btn_search</t>
+  </si>
+  <si>
+    <t>btn_ask_question</t>
+  </si>
+  <si>
+    <t>nav-users</t>
+  </si>
+  <si>
+    <t>nav_bar_users_menu</t>
+  </si>
+  <si>
+    <t>userfilter</t>
+  </si>
+  <si>
+    <t>txt_box_user_search</t>
+  </si>
+  <si>
+    <t>//a[text()='Osanda Deshan']</t>
+  </si>
+  <si>
+    <t>lbl_seach_result</t>
+  </si>
+  <si>
+    <t>//a[@title='How to automate Android 6.0 Date picker to set any date?']</t>
   </si>
 </sst>
 </file>
@@ -139,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -156,6 +183,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1442,10 +1476,438 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IS21"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="253" width="8.85546875" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="8"/>
+      <c r="AU2" s="8"/>
+      <c r="AV2" s="8"/>
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="8"/>
+      <c r="BA2" s="8"/>
+      <c r="BB2" s="8"/>
+      <c r="BC2" s="8"/>
+      <c r="BD2" s="8"/>
+      <c r="BE2" s="8"/>
+      <c r="BF2" s="8"/>
+      <c r="BG2" s="8"/>
+      <c r="BH2" s="8"/>
+      <c r="BI2" s="8"/>
+      <c r="BJ2" s="8"/>
+      <c r="BK2" s="8"/>
+      <c r="BL2" s="8"/>
+      <c r="BM2" s="8"/>
+      <c r="BN2" s="8"/>
+      <c r="BO2" s="8"/>
+      <c r="BP2" s="8"/>
+      <c r="BQ2" s="8"/>
+      <c r="BR2" s="8"/>
+      <c r="BS2" s="8"/>
+      <c r="BT2" s="8"/>
+      <c r="BU2" s="8"/>
+      <c r="BV2" s="8"/>
+      <c r="BW2" s="8"/>
+      <c r="BX2" s="8"/>
+      <c r="BY2" s="8"/>
+      <c r="BZ2" s="8"/>
+      <c r="CA2" s="8"/>
+      <c r="CB2" s="8"/>
+      <c r="CC2" s="8"/>
+      <c r="CD2" s="8"/>
+      <c r="CE2" s="8"/>
+      <c r="CF2" s="8"/>
+      <c r="CG2" s="8"/>
+      <c r="CH2" s="8"/>
+      <c r="CI2" s="8"/>
+      <c r="CJ2" s="8"/>
+      <c r="CK2" s="8"/>
+      <c r="CL2" s="8"/>
+      <c r="CM2" s="8"/>
+      <c r="CN2" s="8"/>
+      <c r="CO2" s="8"/>
+      <c r="CP2" s="8"/>
+      <c r="CQ2" s="8"/>
+      <c r="CR2" s="8"/>
+      <c r="CS2" s="8"/>
+      <c r="CT2" s="8"/>
+      <c r="CU2" s="8"/>
+      <c r="CV2" s="8"/>
+      <c r="CW2" s="8"/>
+      <c r="CX2" s="8"/>
+      <c r="CY2" s="8"/>
+      <c r="CZ2" s="8"/>
+      <c r="DA2" s="8"/>
+      <c r="DB2" s="8"/>
+      <c r="DC2" s="8"/>
+      <c r="DD2" s="8"/>
+      <c r="DE2" s="8"/>
+      <c r="DF2" s="8"/>
+      <c r="DG2" s="8"/>
+      <c r="DH2" s="8"/>
+      <c r="DI2" s="8"/>
+      <c r="DJ2" s="8"/>
+      <c r="DK2" s="8"/>
+      <c r="DL2" s="8"/>
+      <c r="DM2" s="8"/>
+      <c r="DN2" s="8"/>
+      <c r="DO2" s="8"/>
+      <c r="DP2" s="8"/>
+      <c r="DQ2" s="8"/>
+      <c r="DR2" s="8"/>
+      <c r="DS2" s="8"/>
+      <c r="DT2" s="8"/>
+      <c r="DU2" s="8"/>
+      <c r="DV2" s="8"/>
+      <c r="DW2" s="8"/>
+      <c r="DX2" s="8"/>
+      <c r="DY2" s="8"/>
+      <c r="DZ2" s="8"/>
+      <c r="EA2" s="8"/>
+      <c r="EB2" s="8"/>
+      <c r="EC2" s="8"/>
+      <c r="ED2" s="8"/>
+      <c r="EE2" s="8"/>
+      <c r="EF2" s="8"/>
+      <c r="EG2" s="8"/>
+      <c r="EH2" s="8"/>
+      <c r="EI2" s="8"/>
+      <c r="EJ2" s="8"/>
+      <c r="EK2" s="8"/>
+      <c r="EL2" s="8"/>
+      <c r="EM2" s="8"/>
+      <c r="EN2" s="8"/>
+      <c r="EO2" s="8"/>
+      <c r="EP2" s="8"/>
+      <c r="EQ2" s="8"/>
+      <c r="ER2" s="8"/>
+      <c r="ES2" s="8"/>
+      <c r="ET2" s="8"/>
+      <c r="EU2" s="8"/>
+      <c r="EV2" s="8"/>
+      <c r="EW2" s="8"/>
+      <c r="EX2" s="8"/>
+      <c r="EY2" s="8"/>
+      <c r="EZ2" s="8"/>
+      <c r="FA2" s="8"/>
+      <c r="FB2" s="8"/>
+      <c r="FC2" s="8"/>
+      <c r="FD2" s="8"/>
+      <c r="FE2" s="8"/>
+      <c r="FF2" s="8"/>
+      <c r="FG2" s="8"/>
+      <c r="FH2" s="8"/>
+      <c r="FI2" s="8"/>
+      <c r="FJ2" s="8"/>
+      <c r="FK2" s="8"/>
+      <c r="FL2" s="8"/>
+      <c r="FM2" s="8"/>
+      <c r="FN2" s="8"/>
+      <c r="FO2" s="8"/>
+      <c r="FP2" s="8"/>
+      <c r="FQ2" s="8"/>
+      <c r="FR2" s="8"/>
+      <c r="FS2" s="8"/>
+      <c r="FT2" s="8"/>
+      <c r="FU2" s="8"/>
+      <c r="FV2" s="8"/>
+      <c r="FW2" s="8"/>
+      <c r="FX2" s="8"/>
+      <c r="FY2" s="8"/>
+      <c r="FZ2" s="8"/>
+      <c r="GA2" s="8"/>
+      <c r="GB2" s="8"/>
+      <c r="GC2" s="8"/>
+      <c r="GD2" s="8"/>
+      <c r="GE2" s="8"/>
+      <c r="GF2" s="8"/>
+      <c r="GG2" s="8"/>
+      <c r="GH2" s="8"/>
+      <c r="GI2" s="8"/>
+      <c r="GJ2" s="8"/>
+      <c r="GK2" s="8"/>
+      <c r="GL2" s="8"/>
+      <c r="GM2" s="8"/>
+      <c r="GN2" s="8"/>
+      <c r="GO2" s="8"/>
+      <c r="GP2" s="8"/>
+      <c r="GQ2" s="8"/>
+      <c r="GR2" s="8"/>
+      <c r="GS2" s="8"/>
+      <c r="GT2" s="8"/>
+      <c r="GU2" s="8"/>
+      <c r="GV2" s="8"/>
+      <c r="GW2" s="8"/>
+      <c r="GX2" s="8"/>
+      <c r="GY2" s="8"/>
+      <c r="GZ2" s="8"/>
+      <c r="HA2" s="8"/>
+      <c r="HB2" s="8"/>
+      <c r="HC2" s="8"/>
+      <c r="HD2" s="8"/>
+      <c r="HE2" s="8"/>
+      <c r="HF2" s="8"/>
+      <c r="HG2" s="8"/>
+      <c r="HH2" s="8"/>
+      <c r="HI2" s="8"/>
+      <c r="HJ2" s="8"/>
+      <c r="HK2" s="8"/>
+      <c r="HL2" s="8"/>
+      <c r="HM2" s="8"/>
+      <c r="HN2" s="8"/>
+      <c r="HO2" s="8"/>
+      <c r="HP2" s="8"/>
+      <c r="HQ2" s="8"/>
+      <c r="HR2" s="8"/>
+      <c r="HS2" s="8"/>
+      <c r="HT2" s="8"/>
+      <c r="HU2" s="8"/>
+      <c r="HV2" s="8"/>
+      <c r="HW2" s="8"/>
+      <c r="HX2" s="8"/>
+      <c r="HY2" s="8"/>
+      <c r="HZ2" s="8"/>
+      <c r="IA2" s="8"/>
+      <c r="IB2" s="8"/>
+      <c r="IC2" s="8"/>
+      <c r="ID2" s="8"/>
+      <c r="IE2" s="8"/>
+      <c r="IF2" s="8"/>
+      <c r="IG2" s="8"/>
+      <c r="IH2" s="8"/>
+      <c r="II2" s="8"/>
+      <c r="IJ2" s="8"/>
+      <c r="IK2" s="8"/>
+      <c r="IL2" s="8"/>
+      <c r="IM2" s="8"/>
+      <c r="IN2" s="8"/>
+      <c r="IO2" s="8"/>
+      <c r="IP2" s="8"/>
+      <c r="IQ2" s="8"/>
+      <c r="IR2" s="8"/>
+      <c r="IS2" s="8"/>
+    </row>
+    <row r="3" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>LocatorStrategy!$A$2:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B21</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IR20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1468,14 +1930,26 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
+      <c r="A3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1581,159 +2055,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IS20"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="85.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="253" width="8.85546875" style="7" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>LocatorStrategy!$A$2:$A$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B20</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Data Store Implementation and Dynamic Element Implementation is Completed
</commit_message>
<xml_diff>
--- a/resources/locators/locators.xlsx
+++ b/resources/locators/locators.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Element Name</t>
   </si>
@@ -88,6 +88,24 @@
   </si>
   <si>
     <t>//a[@title='How to automate Android 6.0 Date picker to set any date?']</t>
+  </si>
+  <si>
+    <t>test_search_result</t>
+  </si>
+  <si>
+    <t>//a[@title='searchText']</t>
+  </si>
+  <si>
+    <t>//span[@class='-link--channel-name']</t>
+  </si>
+  <si>
+    <t>nav_bar_stackoverflow_menu</t>
+  </si>
+  <si>
+    <t>//a[@class='pl8 js-gps-track nav-links--link']</t>
+  </si>
+  <si>
+    <t>nav_bar_home_menu</t>
   </si>
 </sst>
 </file>
@@ -1479,7 +1497,7 @@
   <dimension ref="A1:IS21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1807,19 +1825,37 @@
       </c>
     </row>
     <row r="7" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="6"/>
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
+      <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="6"/>
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>

</xml_diff>

<commit_message>
Dynamic locator creation updated with data store replacement text. Added new tests
</commit_message>
<xml_diff>
--- a/resources/locators/locators.xlsx
+++ b/resources/locators/locators.xlsx
@@ -2,21 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="669" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" tabRatio="669" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LocatorStrategy" sheetId="31" r:id="rId1"/>
-    <sheet name="HomePage" sheetId="30" r:id="rId2"/>
-    <sheet name="UsersPage" sheetId="32" r:id="rId3"/>
+    <sheet name="LoginPage" sheetId="34" r:id="rId2"/>
+    <sheet name="HomePage" sheetId="30" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Element Name</t>
   </si>
@@ -51,68 +56,47 @@
     <t>Locator Strategy</t>
   </si>
   <si>
-    <t>//input[@name='q']</t>
-  </si>
-  <si>
-    <t>search_bar</t>
-  </si>
-  <si>
-    <t>//a[@href='/questions/ask']</t>
-  </si>
-  <si>
-    <t>//button[@type='submit']//*[@class='svg-icon iconSearch']</t>
-  </si>
-  <si>
-    <t>btn_search</t>
-  </si>
-  <si>
-    <t>btn_ask_question</t>
-  </si>
-  <si>
-    <t>nav-users</t>
-  </si>
-  <si>
-    <t>nav_bar_users_menu</t>
-  </si>
-  <si>
-    <t>userfilter</t>
-  </si>
-  <si>
-    <t>txt_box_user_search</t>
-  </si>
-  <si>
-    <t>//a[text()='Osanda Deshan']</t>
-  </si>
-  <si>
-    <t>lbl_seach_result</t>
-  </si>
-  <si>
-    <t>//a[@title='How to automate Android 6.0 Date picker to set any date?']</t>
-  </si>
-  <si>
-    <t>test_search_result</t>
-  </si>
-  <si>
-    <t>//a[@title='searchText']</t>
-  </si>
-  <si>
-    <t>//span[@class='-link--channel-name']</t>
-  </si>
-  <si>
-    <t>nav_bar_stackoverflow_menu</t>
-  </si>
-  <si>
-    <t>//a[@class='pl8 js-gps-track nav-links--link']</t>
-  </si>
-  <si>
-    <t>nav_bar_home_menu</t>
+    <t>txt_email</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>passwd</t>
+  </si>
+  <si>
+    <t>txt_password</t>
+  </si>
+  <si>
+    <t>nav_bar_signin_link</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'Sign in')]</t>
+  </si>
+  <si>
+    <t>SubmitLogin</t>
+  </si>
+  <si>
+    <t>btn_submit</t>
+  </si>
+  <si>
+    <t>lbl_profile_name</t>
+  </si>
+  <si>
+    <t>//span[text()='profileName']</t>
+  </si>
+  <si>
+    <t>nav_bar_signout_link</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'Sign out')]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -129,6 +113,18 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -181,8 +177,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -209,7 +221,23 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -236,7 +264,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1">
+  <tableStyles count="1" defaultPivotStyle="PivotStyleMedium4">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
@@ -1485,26 +1513,190 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IR20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.85546875" style="8" customWidth="1"/>
+    <col min="4" max="252" width="8.85546875" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>LocatorStrategy!$A$2:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B20</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IS21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="85.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="253" width="8.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1521,13 +1713,13 @@
     </row>
     <row r="2" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -1782,80 +1974,50 @@
     </row>
     <row r="3" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>15</v>
+      <c r="A4" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
@@ -1919,7 +2081,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1934,160 +2096,8 @@
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IR20"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.85546875" style="8" customWidth="1"/>
-    <col min="4" max="252" width="8.85546875" style="8" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>LocatorStrategy!$A$2:$A$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B20</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
Added a login concept and implemented exception handling
</commit_message>
<xml_diff>
--- a/resources/locators/locators.xlsx
+++ b/resources/locators/locators.xlsx
@@ -68,28 +68,28 @@
     <t>txt_password</t>
   </si>
   <si>
+    <t>//a[contains(text(),'Sign in')]</t>
+  </si>
+  <si>
+    <t>SubmitLogin</t>
+  </si>
+  <si>
+    <t>btn_submit</t>
+  </si>
+  <si>
+    <t>lbl_profile_name</t>
+  </si>
+  <si>
+    <t>//span[text()='profileName']</t>
+  </si>
+  <si>
+    <t>nav_bar_signout_link</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'Sign out')]</t>
+  </si>
+  <si>
     <t>nav_bar_signin_link</t>
-  </si>
-  <si>
-    <t>//a[contains(text(),'Sign in')]</t>
-  </si>
-  <si>
-    <t>SubmitLogin</t>
-  </si>
-  <si>
-    <t>btn_submit</t>
-  </si>
-  <si>
-    <t>lbl_profile_name</t>
-  </si>
-  <si>
-    <t>//span[text()='profileName']</t>
-  </si>
-  <si>
-    <t>nav_bar_signout_link</t>
-  </si>
-  <si>
-    <t>//a[contains(text(),'Sign out')]</t>
   </si>
 </sst>
 </file>
@@ -1575,13 +1575,13 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1689,7 +1689,7 @@
   <dimension ref="A1:IS21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1713,13 +1713,13 @@
     </row>
     <row r="2" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -1974,24 +1974,24 @@
     </row>
     <row r="3" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Search test added and did minor modifications
</commit_message>
<xml_diff>
--- a/resources/locators/locators.xlsx
+++ b/resources/locators/locators.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Element Name</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>nav_bar_signin_link</t>
+  </si>
+  <si>
+    <t>search_query_top</t>
+  </si>
+  <si>
+    <t>txt_search_bar</t>
   </si>
 </sst>
 </file>
@@ -1689,7 +1695,7 @@
   <dimension ref="A1:IS21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1995,9 +2001,15 @@
       </c>
     </row>
     <row r="5" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="6"/>
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>

</xml_diff>

<commit_message>
Common steps modified with variables for row operations
</commit_message>
<xml_diff>
--- a/resources/locators/locators.xlsx
+++ b/resources/locators/locators.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Element Name</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>txt_search_bar</t>
+  </si>
+  <si>
+    <t>lbl_search_result</t>
+  </si>
+  <si>
+    <t>//ul[@class='product_list grid row']//a[contains(text(),'searchText')]</t>
   </si>
 </sst>
 </file>
@@ -1695,7 +1701,7 @@
   <dimension ref="A1:IS21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2012,9 +2018,15 @@
       </c>
     </row>
     <row r="6" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
+      <c r="A6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>

</xml_diff>

<commit_message>
Added tests for search dress spec. Removed redundant tests.
</commit_message>
<xml_diff>
--- a/resources/locators/locators.xlsx
+++ b/resources/locators/locators.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>Element Name</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>//ul[@class='product_list grid row']//a[contains(text(),'searchText')]</t>
+  </si>
+  <si>
+    <t>btn_search</t>
+  </si>
+  <si>
+    <t>submit_search</t>
+  </si>
+  <si>
+    <t>//ul[@class='product_list grid row']//a[contains(text(),'Faded Short Sleeve T-shirts')]</t>
+  </si>
+  <si>
+    <t>lbl_search_result_locator</t>
   </si>
 </sst>
 </file>
@@ -1701,7 +1713,7 @@
   <dimension ref="A1:IS21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2029,14 +2041,26 @@
       </c>
     </row>
     <row r="7" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="6"/>
+      <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
+      <c r="A8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:253" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>

</xml_diff>

<commit_message>
Developed the step for open url in new tab
</commit_message>
<xml_diff>
--- a/resources/locators/locators.xlsx
+++ b/resources/locators/locators.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" tabRatio="669" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" tabRatio="669" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LocatorStrategy" sheetId="31" r:id="rId1"/>
     <sheet name="LoginPage" sheetId="34" r:id="rId2"/>
     <sheet name="HomePage" sheetId="30" r:id="rId3"/>
+    <sheet name="UploadPage" sheetId="36" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>Element Name</t>
   </si>
@@ -114,6 +116,42 @@
   </si>
   <si>
     <t>lbl_search_result_locator</t>
+  </si>
+  <si>
+    <t>inputfile</t>
+  </si>
+  <si>
+    <t>//button[contains(text(),'Upload')]</t>
+  </si>
+  <si>
+    <t>uploadfile_0</t>
+  </si>
+  <si>
+    <t>terms</t>
+  </si>
+  <si>
+    <t>send</t>
+  </si>
+  <si>
+    <t>//*[contains(text(), '1 file')]</t>
+  </si>
+  <si>
+    <t>lbl_upload_success</t>
+  </si>
+  <si>
+    <t>btn_upload_file</t>
+  </si>
+  <si>
+    <t>btn_terms</t>
+  </si>
+  <si>
+    <t>btn_test_upload</t>
+  </si>
+  <si>
+    <t>btn_upload</t>
+  </si>
+  <si>
+    <t>btn_choose_file</t>
   </si>
 </sst>
 </file>
@@ -1712,7 +1750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IS21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -2149,4 +2187,176 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IS21"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="253" width="8.85546875" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>